<commit_message>
complete validation. next logic for saving sim data
</commit_message>
<xml_diff>
--- a/powerapp/data/assignment_ufls.xlsx
+++ b/powerapp/data/assignment_ufls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myIjat\Dojo\power_app\powerapp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/externalDrive/code-gym/work/powerapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37251B2-29EC-4C0A-AA4E-A8E1792E6273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98780BF-5165-C74C-8DA6-13979AD6D7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{EAAC684E-7C1B-4F2F-BC7C-B97D8EF3A83B}"/>
+    <workbookView xWindow="-19220" yWindow="600" windowWidth="19220" windowHeight="21000" xr2:uid="{EAAC684E-7C1B-4F2F-BC7C-B97D8EF3A83B}"/>
   </bookViews>
   <sheets>
     <sheet name="ufls_assignment" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1022,21 +1022,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F1E9AA-42FA-48CE-9C0D-6753CE8DE448}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C607"/>
+  <dimension ref="A1:D607"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.5" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>171</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>174</v>
       </c>
@@ -1056,7 +1055,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" hidden="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>175</v>
       </c>
@@ -1066,8 +1065,9 @@
       <c r="C3" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" hidden="1">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>176</v>
       </c>
@@ -1077,8 +1077,9 @@
       <c r="C4" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" hidden="1">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>177</v>
       </c>
@@ -1088,8 +1089,9 @@
       <c r="C5" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" hidden="1">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>178</v>
       </c>
@@ -1099,8 +1101,9 @@
       <c r="C6" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" hidden="1">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>179</v>
       </c>
@@ -1110,8 +1113,9 @@
       <c r="C7" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" hidden="1">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>180</v>
       </c>
@@ -1121,8 +1125,9 @@
       <c r="C8" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" hidden="1">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>181</v>
       </c>
@@ -1132,8 +1137,9 @@
       <c r="C9" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" hidden="1">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>188</v>
       </c>
@@ -1143,8 +1149,9 @@
       <c r="C10" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" hidden="1">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>182</v>
       </c>
@@ -1154,8 +1161,9 @@
       <c r="C11" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" hidden="1">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>183</v>
       </c>
@@ -1165,8 +1173,9 @@
       <c r="C12" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" hidden="1">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>184</v>
       </c>
@@ -1176,8 +1185,9 @@
       <c r="C13" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" hidden="1">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>189</v>
       </c>
@@ -1187,8 +1197,9 @@
       <c r="C14" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" hidden="1">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>185</v>
       </c>
@@ -1199,7 +1210,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>186</v>
       </c>
@@ -1210,7 +1221,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1230,7 @@
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" hidden="1">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
@@ -1228,7 +1239,7 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" hidden="1">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1237,7 +1248,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" hidden="1">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1257,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" hidden="1">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1255,7 +1266,7 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" hidden="1">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -1264,7 +1275,7 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" hidden="1">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1284,7 @@
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" s="6" customFormat="1" hidden="1">
+    <row r="24" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1284,7 +1295,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="6" customFormat="1" hidden="1">
+    <row r="25" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1304,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="26" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +1315,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="27" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>10</v>
       </c>
@@ -1315,7 +1326,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="28" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1326,7 +1337,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="29" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
@@ -1335,7 +1346,7 @@
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" hidden="1">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -1346,7 +1357,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -1357,7 +1368,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -1368,7 +1379,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -1377,7 +1388,7 @@
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" hidden="1">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1399,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>19</v>
       </c>
@@ -1410,7 +1421,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
@@ -1419,7 +1430,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" hidden="1">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
@@ -1430,7 +1441,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>22</v>
       </c>
@@ -1441,7 +1452,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>23</v>
       </c>
@@ -1452,7 +1463,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>24</v>
       </c>
@@ -1461,7 +1472,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" hidden="1">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>25</v>
       </c>
@@ -1470,7 +1481,7 @@
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" hidden="1">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>26</v>
       </c>
@@ -1481,7 +1492,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>27</v>
       </c>
@@ -1490,7 +1501,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" hidden="1">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>28</v>
       </c>
@@ -1499,7 +1510,7 @@
       </c>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" hidden="1">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>29</v>
       </c>
@@ -1510,7 +1521,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>30</v>
       </c>
@@ -1519,7 +1530,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" hidden="1">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>31</v>
       </c>
@@ -1528,7 +1539,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" hidden="1">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>32</v>
       </c>
@@ -1537,7 +1548,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="15" hidden="1" customHeight="1">
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>33</v>
       </c>
@@ -1546,7 +1557,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="15" hidden="1" customHeight="1">
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>34</v>
       </c>
@@ -1555,7 +1566,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" hidden="1">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>35</v>
       </c>
@@ -1564,7 +1575,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3" hidden="1">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>36</v>
       </c>
@@ -1573,7 +1584,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" hidden="1">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>37</v>
       </c>
@@ -1582,7 +1593,7 @@
       </c>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" hidden="1">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>38</v>
       </c>
@@ -1591,7 +1602,7 @@
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" hidden="1">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>173</v>
       </c>
@@ -1600,7 +1611,7 @@
       </c>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:3" hidden="1">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>39</v>
       </c>
@@ -1609,7 +1620,7 @@
       </c>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" hidden="1">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>40</v>
       </c>
@@ -1618,7 +1629,7 @@
       </c>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" hidden="1">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>41</v>
       </c>
@@ -1627,7 +1638,7 @@
       </c>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:3" hidden="1">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>42</v>
       </c>
@@ -1636,7 +1647,7 @@
       </c>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>43</v>
       </c>
@@ -1647,7 +1658,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>44</v>
       </c>
@@ -1656,7 +1667,7 @@
       </c>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3" hidden="1">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>45</v>
       </c>
@@ -1665,7 +1676,7 @@
       </c>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3" hidden="1">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>46</v>
       </c>
@@ -1674,7 +1685,7 @@
       </c>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" spans="1:3" hidden="1">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>47</v>
       </c>
@@ -1683,7 +1694,7 @@
       </c>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" spans="1:3" hidden="1">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>48</v>
       </c>
@@ -1694,7 +1705,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>49</v>
       </c>
@@ -1705,7 +1716,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>50</v>
       </c>
@@ -1714,7 +1725,7 @@
       </c>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3" hidden="1">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>51</v>
       </c>
@@ -1723,7 +1734,7 @@
       </c>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3" hidden="1">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>52</v>
       </c>
@@ -1734,7 +1745,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>53</v>
       </c>
@@ -1743,7 +1754,7 @@
       </c>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3" hidden="1">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>54</v>
       </c>
@@ -1752,7 +1763,7 @@
       </c>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3" hidden="1">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>55</v>
       </c>
@@ -1761,7 +1772,7 @@
       </c>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3" hidden="1">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>56</v>
       </c>
@@ -1770,7 +1781,7 @@
       </c>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3" hidden="1">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -1779,7 +1790,7 @@
       </c>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3" hidden="1">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>58</v>
       </c>
@@ -1790,7 +1801,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>59</v>
       </c>
@@ -1799,7 +1810,7 @@
       </c>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3" hidden="1">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>60</v>
       </c>
@@ -1808,7 +1819,7 @@
       </c>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3" hidden="1">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>61</v>
       </c>
@@ -1817,7 +1828,7 @@
       </c>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3" hidden="1">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>62</v>
       </c>
@@ -1828,7 +1839,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>63</v>
       </c>
@@ -1837,7 +1848,7 @@
       </c>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3" hidden="1">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>64</v>
       </c>
@@ -1846,7 +1857,7 @@
       </c>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="1:3" hidden="1">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>65</v>
       </c>
@@ -1857,7 +1868,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>66</v>
       </c>
@@ -1866,7 +1877,7 @@
       </c>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" spans="1:3" hidden="1">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>67</v>
       </c>
@@ -1875,7 +1886,7 @@
       </c>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:3" hidden="1">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>68</v>
       </c>
@@ -1884,7 +1895,7 @@
       </c>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:3" hidden="1">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>69</v>
       </c>
@@ -1893,7 +1904,7 @@
       </c>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" spans="1:3" hidden="1">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>70</v>
       </c>
@@ -1902,7 +1913,7 @@
       </c>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" spans="1:3" hidden="1">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>71</v>
       </c>
@@ -1913,7 +1924,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>72</v>
       </c>
@@ -1924,7 +1935,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>73</v>
       </c>
@@ -1933,7 +1944,7 @@
       </c>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:3" hidden="1">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>74</v>
       </c>
@@ -1942,7 +1953,7 @@
       </c>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:3" hidden="1">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>75</v>
       </c>
@@ -1951,7 +1962,7 @@
       </c>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:3" hidden="1">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>76</v>
       </c>
@@ -1960,7 +1971,7 @@
       </c>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:3" hidden="1">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>156</v>
       </c>
@@ -1969,7 +1980,7 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:3" hidden="1">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>77</v>
       </c>
@@ -1978,7 +1989,7 @@
       </c>
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="1:3" hidden="1">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>78</v>
       </c>
@@ -1987,7 +1998,7 @@
       </c>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="1:3" hidden="1">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>79</v>
       </c>
@@ -1996,7 +2007,7 @@
       </c>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="1:3" hidden="1">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>80</v>
       </c>
@@ -2007,7 +2018,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>81</v>
       </c>
@@ -2016,7 +2027,7 @@
       </c>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3" hidden="1">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>82</v>
       </c>
@@ -2025,7 +2036,7 @@
       </c>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="1:3" hidden="1">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>83</v>
       </c>
@@ -2034,7 +2045,7 @@
       </c>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="103" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>84</v>
       </c>
@@ -2043,7 +2054,7 @@
       </c>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="104" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>85</v>
       </c>
@@ -2054,7 +2065,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="105" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>86</v>
       </c>
@@ -2063,7 +2074,7 @@
       </c>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="1:3" hidden="1">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>87</v>
       </c>
@@ -2072,7 +2083,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" hidden="1">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>88</v>
       </c>
@@ -2081,7 +2092,7 @@
       </c>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" spans="1:3" hidden="1">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>89</v>
       </c>
@@ -2090,7 +2101,7 @@
       </c>
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="1:3" hidden="1">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>90</v>
       </c>
@@ -2099,7 +2110,7 @@
       </c>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="1:3" hidden="1">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>91</v>
       </c>
@@ -2108,7 +2119,7 @@
       </c>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="1:3" hidden="1">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>92</v>
       </c>
@@ -2117,7 +2128,7 @@
       </c>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" spans="1:3" hidden="1">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>93</v>
       </c>
@@ -2128,7 +2139,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>94</v>
       </c>
@@ -2139,7 +2150,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>95</v>
       </c>
@@ -2148,7 +2159,7 @@
       </c>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="115" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>96</v>
       </c>
@@ -2157,7 +2168,7 @@
       </c>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="116" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>97</v>
       </c>
@@ -2166,7 +2177,7 @@
       </c>
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="1:3" hidden="1">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>98</v>
       </c>
@@ -2175,7 +2186,7 @@
       </c>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:3" hidden="1">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>99</v>
       </c>
@@ -2184,7 +2195,7 @@
       </c>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="1:3" hidden="1">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>170</v>
       </c>
@@ -2195,7 +2206,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>100</v>
       </c>
@@ -2204,7 +2215,7 @@
       </c>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:3" hidden="1">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>101</v>
       </c>
@@ -2215,7 +2226,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>102</v>
       </c>
@@ -2226,7 +2237,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>103</v>
       </c>
@@ -2235,7 +2246,7 @@
       </c>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="1:3" hidden="1">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>104</v>
       </c>
@@ -2244,7 +2255,7 @@
       </c>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="1:3" hidden="1">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>105</v>
       </c>
@@ -2255,7 +2266,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>106</v>
       </c>
@@ -2264,7 +2275,7 @@
       </c>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="1:3" hidden="1">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>107</v>
       </c>
@@ -2273,7 +2284,7 @@
       </c>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="1:3" hidden="1">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>108</v>
       </c>
@@ -2282,7 +2293,7 @@
       </c>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="1:3" hidden="1">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>109</v>
       </c>
@@ -2291,7 +2302,7 @@
       </c>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="1:3" hidden="1">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>110</v>
       </c>
@@ -2302,7 +2313,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>111</v>
       </c>
@@ -2311,7 +2322,7 @@
       </c>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="1:3" hidden="1">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>112</v>
       </c>
@@ -2320,7 +2331,7 @@
       </c>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" spans="1:3" hidden="1">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>172</v>
       </c>
@@ -2331,7 +2342,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>113</v>
       </c>
@@ -2340,7 +2351,7 @@
       </c>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="1:3" hidden="1">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>114</v>
       </c>
@@ -2351,7 +2362,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>115</v>
       </c>
@@ -2362,7 +2373,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>116</v>
       </c>
@@ -2373,7 +2384,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>117</v>
       </c>
@@ -2384,7 +2395,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>118</v>
       </c>
@@ -2395,7 +2406,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>119</v>
       </c>
@@ -2406,7 +2417,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>120</v>
       </c>
@@ -2417,7 +2428,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>121</v>
       </c>
@@ -2428,7 +2439,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>122</v>
       </c>
@@ -2439,7 +2450,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>123</v>
       </c>
@@ -2450,7 +2461,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>124</v>
       </c>
@@ -2461,7 +2472,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>125</v>
       </c>
@@ -2472,7 +2483,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>126</v>
       </c>
@@ -2483,7 +2494,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="148" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="148" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>127</v>
       </c>
@@ -2494,7 +2505,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="149" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="149" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>128</v>
       </c>
@@ -2505,7 +2516,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="150" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="150" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>129</v>
       </c>
@@ -2516,7 +2527,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="151" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="151" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>130</v>
       </c>
@@ -2527,7 +2538,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>131</v>
       </c>
@@ -2538,7 +2549,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>132</v>
       </c>
@@ -2549,7 +2560,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>133</v>
       </c>
@@ -2560,7 +2571,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>134</v>
       </c>
@@ -2571,7 +2582,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>135</v>
       </c>
@@ -2582,7 +2593,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>136</v>
       </c>
@@ -2593,7 +2604,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>137</v>
       </c>
@@ -2604,7 +2615,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="159" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="159" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>138</v>
       </c>
@@ -2615,7 +2626,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="160" spans="1:3" s="7" customFormat="1" hidden="1">
+    <row r="160" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>139</v>
       </c>
@@ -2626,7 +2637,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>140</v>
       </c>
@@ -2637,7 +2648,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>141</v>
       </c>
@@ -2648,7 +2659,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>142</v>
       </c>
@@ -2659,7 +2670,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>143</v>
       </c>
@@ -2670,7 +2681,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>144</v>
       </c>
@@ -2681,7 +2692,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="166" spans="1:3" hidden="1">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>145</v>
       </c>
@@ -2692,7 +2703,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>146</v>
       </c>
@@ -2703,7 +2714,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="168" spans="1:3" hidden="1">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>147</v>
       </c>
@@ -2714,7 +2725,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>148</v>
       </c>
@@ -2725,7 +2736,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170" spans="1:3" hidden="1">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>149</v>
       </c>
@@ -2736,7 +2747,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>150</v>
       </c>
@@ -2747,7 +2758,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>151</v>
       </c>
@@ -2758,7 +2769,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>152</v>
       </c>
@@ -2769,7 +2780,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>187</v>
       </c>
@@ -2780,7 +2791,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="175" spans="1:3" hidden="1">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>153</v>
       </c>
@@ -2791,7 +2802,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>154</v>
       </c>
@@ -2802,7 +2813,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>155</v>
       </c>
@@ -2813,2166 +2824,2160 @@
         <v>169</v>
       </c>
     </row>
-    <row r="178" spans="1:3" s="7" customFormat="1">
+    <row r="178" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178"/>
       <c r="B178"/>
       <c r="C178"/>
     </row>
-    <row r="179" spans="1:3" s="7" customFormat="1">
+    <row r="179" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179"/>
       <c r="B179"/>
       <c r="C179"/>
     </row>
-    <row r="180" spans="1:3" s="7" customFormat="1">
+    <row r="180" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180"/>
       <c r="B180"/>
       <c r="C180"/>
     </row>
-    <row r="181" spans="1:3" s="7" customFormat="1">
+    <row r="181" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181"/>
       <c r="B181"/>
       <c r="C181"/>
     </row>
-    <row r="182" spans="1:3" s="7" customFormat="1">
+    <row r="182" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182"/>
       <c r="B182"/>
       <c r="C182"/>
     </row>
-    <row r="183" spans="1:3" s="7" customFormat="1">
+    <row r="183" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183"/>
       <c r="B183"/>
       <c r="C183"/>
     </row>
-    <row r="184" spans="1:3" s="7" customFormat="1">
+    <row r="184" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184"/>
       <c r="B184"/>
       <c r="C184"/>
     </row>
-    <row r="185" spans="1:3" s="7" customFormat="1">
+    <row r="185" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185"/>
       <c r="B185"/>
       <c r="C185"/>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186"/>
       <c r="B186"/>
       <c r="C186"/>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187"/>
       <c r="B187"/>
       <c r="C187"/>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188"/>
       <c r="B188"/>
       <c r="C188"/>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189"/>
       <c r="B189"/>
       <c r="C189"/>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190"/>
       <c r="B190"/>
       <c r="C190"/>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191"/>
       <c r="B191"/>
       <c r="C191"/>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192"/>
       <c r="B192"/>
       <c r="C192"/>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193"/>
       <c r="B193"/>
       <c r="C193"/>
     </row>
-    <row r="194" spans="1:3" s="7" customFormat="1">
+    <row r="194" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194"/>
       <c r="B194"/>
       <c r="C194"/>
     </row>
-    <row r="195" spans="1:3" s="7" customFormat="1">
+    <row r="195" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195"/>
       <c r="B195"/>
       <c r="C195"/>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196"/>
       <c r="B196"/>
       <c r="C196"/>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197"/>
       <c r="B197"/>
       <c r="C197"/>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198"/>
       <c r="B198"/>
       <c r="C198"/>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199"/>
       <c r="B199"/>
       <c r="C199"/>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200"/>
       <c r="B200"/>
       <c r="C200"/>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201"/>
       <c r="B201"/>
       <c r="C201"/>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202"/>
       <c r="B202"/>
       <c r="C202"/>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203"/>
       <c r="B203"/>
       <c r="C203"/>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204"/>
       <c r="B204"/>
       <c r="C204"/>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205"/>
       <c r="B205"/>
       <c r="C205"/>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206"/>
       <c r="B206"/>
       <c r="C206"/>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207"/>
       <c r="B207"/>
       <c r="C207"/>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208"/>
       <c r="B208"/>
       <c r="C208"/>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209"/>
       <c r="B209"/>
       <c r="C209"/>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210"/>
       <c r="B210"/>
       <c r="C210"/>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211"/>
       <c r="B211"/>
       <c r="C211"/>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212"/>
       <c r="B212"/>
       <c r="C212"/>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213"/>
       <c r="B213"/>
       <c r="C213"/>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214"/>
       <c r="B214"/>
       <c r="C214"/>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215"/>
       <c r="B215"/>
       <c r="C215"/>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216"/>
       <c r="B216"/>
       <c r="C216"/>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217"/>
       <c r="B217"/>
       <c r="C217"/>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218"/>
       <c r="B218"/>
       <c r="C218"/>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219"/>
       <c r="B219"/>
       <c r="C219"/>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220"/>
       <c r="B220"/>
       <c r="C220"/>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221"/>
       <c r="B221"/>
       <c r="C221"/>
     </row>
-    <row r="222" spans="1:3" s="7" customFormat="1">
+    <row r="222" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222"/>
       <c r="B222"/>
       <c r="C222"/>
     </row>
-    <row r="223" spans="1:3" s="7" customFormat="1">
+    <row r="223" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223"/>
       <c r="B223"/>
       <c r="C223"/>
     </row>
-    <row r="224" spans="1:3" s="7" customFormat="1">
+    <row r="224" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224"/>
       <c r="B224"/>
       <c r="C224"/>
     </row>
-    <row r="225" spans="1:3" s="7" customFormat="1">
+    <row r="225" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225"/>
       <c r="B225"/>
       <c r="C225"/>
     </row>
-    <row r="226" spans="1:3" s="7" customFormat="1">
+    <row r="226" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226"/>
       <c r="B226"/>
       <c r="C226"/>
     </row>
-    <row r="227" spans="1:3" s="7" customFormat="1">
+    <row r="227" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227"/>
       <c r="B227"/>
       <c r="C227"/>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228"/>
       <c r="B228"/>
       <c r="C228"/>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229"/>
       <c r="B229"/>
       <c r="C229"/>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230"/>
       <c r="B230"/>
       <c r="C230"/>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231"/>
       <c r="B231"/>
       <c r="C231"/>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232"/>
       <c r="B232"/>
       <c r="C232"/>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233"/>
       <c r="B233"/>
       <c r="C233"/>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234"/>
       <c r="B234"/>
       <c r="C234"/>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235"/>
       <c r="B235"/>
       <c r="C235"/>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236"/>
       <c r="B236"/>
       <c r="C236"/>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237"/>
       <c r="B237"/>
       <c r="C237"/>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238"/>
       <c r="B238"/>
       <c r="C238"/>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239"/>
       <c r="B239"/>
       <c r="C239"/>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240"/>
       <c r="B240"/>
       <c r="C240"/>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241"/>
       <c r="B241"/>
       <c r="C241"/>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242"/>
       <c r="B242"/>
       <c r="C242"/>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243"/>
       <c r="B243"/>
       <c r="C243"/>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244"/>
       <c r="B244"/>
       <c r="C244"/>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245"/>
       <c r="B245"/>
       <c r="C245"/>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246"/>
       <c r="B246"/>
       <c r="C246"/>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247"/>
       <c r="B247"/>
       <c r="C247"/>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248"/>
       <c r="B248"/>
       <c r="C248"/>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249"/>
       <c r="B249"/>
       <c r="C249"/>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250"/>
       <c r="B250"/>
       <c r="C250"/>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251"/>
       <c r="B251"/>
       <c r="C251"/>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252"/>
       <c r="B252"/>
       <c r="C252"/>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253"/>
       <c r="B253"/>
       <c r="C253"/>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254"/>
       <c r="B254"/>
       <c r="C254"/>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255"/>
       <c r="B255"/>
       <c r="C255"/>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256"/>
       <c r="B256"/>
       <c r="C256"/>
     </row>
-    <row r="257" spans="1:3" s="7" customFormat="1">
+    <row r="257" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257"/>
       <c r="B257"/>
       <c r="C257"/>
     </row>
-    <row r="258" spans="1:3" s="7" customFormat="1">
+    <row r="258" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258"/>
       <c r="B258"/>
       <c r="C258"/>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259"/>
       <c r="B259"/>
       <c r="C259"/>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260"/>
       <c r="B260"/>
       <c r="C260"/>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261"/>
       <c r="B261"/>
       <c r="C261"/>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262"/>
       <c r="B262"/>
       <c r="C262"/>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263"/>
       <c r="B263"/>
       <c r="C263"/>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264"/>
       <c r="B264"/>
       <c r="C264"/>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265"/>
       <c r="B265"/>
       <c r="C265"/>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266"/>
       <c r="B266"/>
       <c r="C266"/>
     </row>
-    <row r="267" spans="1:3" ht="14.5" customHeight="1">
+    <row r="267" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267"/>
       <c r="B267"/>
       <c r="C267"/>
     </row>
-    <row r="268" spans="1:3" ht="14.5" customHeight="1">
+    <row r="268" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268"/>
       <c r="B268"/>
       <c r="C268"/>
     </row>
-    <row r="269" spans="1:3" ht="14.5" customHeight="1">
+    <row r="269" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269"/>
       <c r="B269"/>
       <c r="C269"/>
     </row>
-    <row r="270" spans="1:3" ht="14.5" customHeight="1">
+    <row r="270" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270"/>
       <c r="B270"/>
       <c r="C270"/>
     </row>
-    <row r="271" spans="1:3" ht="14.5" customHeight="1">
+    <row r="271" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271"/>
       <c r="B271"/>
       <c r="C271"/>
     </row>
-    <row r="272" spans="1:3" ht="14.5" customHeight="1">
+    <row r="272" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272"/>
       <c r="B272"/>
       <c r="C272"/>
     </row>
-    <row r="273" spans="1:3" ht="14.5" customHeight="1">
+    <row r="273" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273"/>
       <c r="B273"/>
       <c r="C273"/>
     </row>
-    <row r="274" spans="1:3" ht="14.5" customHeight="1">
+    <row r="274" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274"/>
       <c r="B274"/>
       <c r="C274"/>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275"/>
       <c r="B275"/>
       <c r="C275"/>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276"/>
       <c r="B276"/>
       <c r="C276"/>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277"/>
       <c r="B277"/>
       <c r="C277"/>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278"/>
       <c r="B278"/>
       <c r="C278"/>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279"/>
       <c r="B279"/>
       <c r="C279"/>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280"/>
       <c r="B280"/>
       <c r="C280"/>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281"/>
       <c r="B281"/>
       <c r="C281"/>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282"/>
       <c r="B282"/>
       <c r="C282"/>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283"/>
       <c r="B283"/>
       <c r="C283"/>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284"/>
       <c r="B284"/>
       <c r="C284"/>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285"/>
       <c r="B285"/>
       <c r="C285"/>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286"/>
       <c r="B286"/>
       <c r="C286"/>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287"/>
       <c r="B287"/>
       <c r="C287"/>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288"/>
       <c r="B288"/>
       <c r="C288"/>
     </row>
-    <row r="289" spans="1:3" s="7" customFormat="1">
+    <row r="289" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A289"/>
       <c r="B289"/>
       <c r="C289"/>
     </row>
-    <row r="290" spans="1:3" s="7" customFormat="1">
+    <row r="290" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A290"/>
       <c r="B290"/>
       <c r="C290"/>
     </row>
-    <row r="291" spans="1:3" s="7" customFormat="1">
+    <row r="291" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291"/>
       <c r="B291"/>
       <c r="C291"/>
     </row>
-    <row r="292" spans="1:3" s="7" customFormat="1">
+    <row r="292" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A292"/>
       <c r="B292"/>
       <c r="C292"/>
     </row>
-    <row r="293" spans="1:3" s="7" customFormat="1">
+    <row r="293" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A293"/>
       <c r="B293"/>
       <c r="C293"/>
     </row>
-    <row r="294" spans="1:3" s="7" customFormat="1">
+    <row r="294" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A294"/>
       <c r="B294"/>
       <c r="C294"/>
     </row>
-    <row r="295" spans="1:3" s="7" customFormat="1">
+    <row r="295" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A295"/>
       <c r="B295"/>
       <c r="C295"/>
     </row>
-    <row r="296" spans="1:3" s="7" customFormat="1">
+    <row r="296" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A296"/>
       <c r="B296"/>
       <c r="C296"/>
     </row>
-    <row r="297" spans="1:3" s="7" customFormat="1">
+    <row r="297" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A297"/>
       <c r="B297"/>
       <c r="C297"/>
     </row>
-    <row r="298" spans="1:3" s="7" customFormat="1">
+    <row r="298" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A298"/>
       <c r="B298"/>
       <c r="C298"/>
     </row>
-    <row r="299" spans="1:3" s="7" customFormat="1">
+    <row r="299" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A299"/>
       <c r="B299"/>
       <c r="C299"/>
     </row>
-    <row r="300" spans="1:3" s="7" customFormat="1">
+    <row r="300" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A300"/>
       <c r="B300"/>
       <c r="C300"/>
     </row>
-    <row r="301" spans="1:3" s="7" customFormat="1">
+    <row r="301" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A301"/>
       <c r="B301"/>
       <c r="C301"/>
     </row>
-    <row r="302" spans="1:3" s="7" customFormat="1">
+    <row r="302" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A302"/>
       <c r="B302"/>
       <c r="C302"/>
     </row>
-    <row r="303" spans="1:3" s="7" customFormat="1">
+    <row r="303" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A303"/>
       <c r="B303"/>
       <c r="C303"/>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304"/>
       <c r="B304"/>
       <c r="C304"/>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305"/>
       <c r="B305"/>
       <c r="C305"/>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306"/>
       <c r="B306"/>
       <c r="C306"/>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307"/>
       <c r="B307"/>
       <c r="C307"/>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308"/>
       <c r="B308"/>
       <c r="C308"/>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309"/>
       <c r="B309"/>
       <c r="C309"/>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310"/>
       <c r="B310"/>
       <c r="C310"/>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311"/>
       <c r="B311"/>
       <c r="C311"/>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312"/>
       <c r="B312"/>
       <c r="C312"/>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313"/>
       <c r="B313"/>
       <c r="C313"/>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314"/>
       <c r="B314"/>
       <c r="C314"/>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315"/>
       <c r="B315"/>
       <c r="C315"/>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316"/>
       <c r="B316"/>
       <c r="C316"/>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317"/>
       <c r="B317"/>
       <c r="C317"/>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318"/>
       <c r="B318"/>
       <c r="C318"/>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319"/>
       <c r="B319"/>
       <c r="C319"/>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320"/>
       <c r="B320"/>
       <c r="C320"/>
     </row>
-    <row r="321" spans="1:3">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321"/>
       <c r="B321"/>
       <c r="C321"/>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322"/>
       <c r="B322"/>
       <c r="C322"/>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323"/>
       <c r="B323"/>
       <c r="C323"/>
     </row>
-    <row r="324" spans="1:3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324"/>
       <c r="B324"/>
       <c r="C324"/>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325"/>
       <c r="B325"/>
       <c r="C325"/>
     </row>
-    <row r="326" spans="1:3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326"/>
       <c r="B326"/>
       <c r="C326"/>
     </row>
-    <row r="327" spans="1:3">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327"/>
       <c r="B327"/>
       <c r="C327"/>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328"/>
       <c r="B328"/>
       <c r="C328"/>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329"/>
       <c r="B329"/>
       <c r="C329"/>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330"/>
       <c r="B330"/>
       <c r="C330"/>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331"/>
       <c r="B331"/>
       <c r="C331"/>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332"/>
       <c r="B332"/>
       <c r="C332"/>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333"/>
       <c r="B333"/>
       <c r="C333"/>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334"/>
       <c r="B334"/>
       <c r="C334"/>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335"/>
       <c r="B335"/>
       <c r="C335"/>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336"/>
       <c r="B336"/>
       <c r="C336"/>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337"/>
       <c r="B337"/>
       <c r="C337"/>
     </row>
-    <row r="338" spans="1:3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338"/>
       <c r="B338"/>
       <c r="C338"/>
     </row>
-    <row r="339" spans="1:3">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339"/>
       <c r="B339"/>
       <c r="C339"/>
     </row>
-    <row r="340" spans="1:3">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340"/>
       <c r="B340"/>
       <c r="C340"/>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341"/>
       <c r="B341"/>
       <c r="C341"/>
     </row>
-    <row r="342" spans="1:3">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342"/>
       <c r="B342"/>
       <c r="C342"/>
     </row>
-    <row r="343" spans="1:3">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343"/>
       <c r="B343"/>
       <c r="C343"/>
     </row>
-    <row r="344" spans="1:3">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344"/>
       <c r="B344"/>
       <c r="C344"/>
     </row>
-    <row r="345" spans="1:3">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345"/>
       <c r="B345"/>
       <c r="C345"/>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346"/>
       <c r="B346"/>
       <c r="C346"/>
     </row>
-    <row r="347" spans="1:3">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347"/>
       <c r="B347"/>
       <c r="C347"/>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348"/>
       <c r="B348"/>
       <c r="C348"/>
     </row>
-    <row r="349" spans="1:3">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349"/>
       <c r="B349"/>
       <c r="C349"/>
     </row>
-    <row r="350" spans="1:3">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350"/>
       <c r="B350"/>
       <c r="C350"/>
     </row>
-    <row r="351" spans="1:3">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351"/>
       <c r="B351"/>
       <c r="C351"/>
     </row>
-    <row r="352" spans="1:3">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352"/>
       <c r="B352"/>
       <c r="C352"/>
     </row>
-    <row r="353" spans="1:3" s="7" customFormat="1">
+    <row r="353" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A353"/>
       <c r="B353"/>
       <c r="C353"/>
     </row>
-    <row r="354" spans="1:3">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354"/>
       <c r="B354"/>
       <c r="C354"/>
     </row>
-    <row r="355" spans="1:3">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355"/>
       <c r="B355"/>
       <c r="C355"/>
     </row>
-    <row r="356" spans="1:3">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356"/>
       <c r="B356"/>
       <c r="C356"/>
     </row>
-    <row r="357" spans="1:3">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357"/>
       <c r="B357"/>
       <c r="C357"/>
     </row>
-    <row r="358" spans="1:3">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358"/>
       <c r="B358"/>
       <c r="C358"/>
     </row>
-    <row r="359" spans="1:3">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359"/>
       <c r="B359"/>
       <c r="C359"/>
     </row>
-    <row r="360" spans="1:3">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360"/>
       <c r="B360"/>
       <c r="C360"/>
     </row>
-    <row r="361" spans="1:3">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361"/>
       <c r="B361"/>
       <c r="C361"/>
     </row>
-    <row r="362" spans="1:3" s="7" customFormat="1">
+    <row r="362" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362"/>
       <c r="B362"/>
       <c r="C362"/>
     </row>
-    <row r="363" spans="1:3">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A363"/>
       <c r="B363"/>
       <c r="C363"/>
     </row>
-    <row r="364" spans="1:3">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364"/>
       <c r="B364"/>
       <c r="C364"/>
     </row>
-    <row r="365" spans="1:3">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365"/>
       <c r="B365"/>
       <c r="C365"/>
     </row>
-    <row r="366" spans="1:3">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366"/>
       <c r="B366"/>
       <c r="C366"/>
     </row>
-    <row r="367" spans="1:3">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367"/>
       <c r="B367"/>
       <c r="C367"/>
     </row>
-    <row r="368" spans="1:3">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368"/>
       <c r="B368"/>
       <c r="C368"/>
     </row>
-    <row r="369" spans="1:3">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369"/>
       <c r="B369"/>
       <c r="C369"/>
     </row>
-    <row r="370" spans="1:3">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370"/>
       <c r="B370"/>
       <c r="C370"/>
     </row>
-    <row r="371" spans="1:3">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371"/>
       <c r="B371"/>
       <c r="C371"/>
     </row>
-    <row r="372" spans="1:3">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372"/>
       <c r="B372"/>
       <c r="C372"/>
     </row>
-    <row r="373" spans="1:3">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373"/>
       <c r="B373"/>
       <c r="C373"/>
     </row>
-    <row r="374" spans="1:3">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374"/>
       <c r="B374"/>
       <c r="C374"/>
     </row>
-    <row r="375" spans="1:3">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375"/>
       <c r="B375"/>
       <c r="C375"/>
     </row>
-    <row r="376" spans="1:3">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376"/>
       <c r="B376"/>
       <c r="C376"/>
     </row>
-    <row r="377" spans="1:3">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377"/>
       <c r="B377"/>
       <c r="C377"/>
     </row>
-    <row r="378" spans="1:3">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378"/>
       <c r="B378"/>
       <c r="C378"/>
     </row>
-    <row r="379" spans="1:3">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379"/>
       <c r="B379"/>
       <c r="C379"/>
     </row>
-    <row r="380" spans="1:3">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380"/>
       <c r="B380"/>
       <c r="C380"/>
     </row>
-    <row r="381" spans="1:3">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381"/>
       <c r="B381"/>
       <c r="C381"/>
     </row>
-    <row r="382" spans="1:3">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382"/>
       <c r="B382"/>
       <c r="C382"/>
     </row>
-    <row r="383" spans="1:3">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383"/>
       <c r="B383"/>
       <c r="C383"/>
     </row>
-    <row r="384" spans="1:3">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384"/>
       <c r="B384"/>
       <c r="C384"/>
     </row>
-    <row r="385" spans="1:3">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385"/>
       <c r="B385"/>
       <c r="C385"/>
     </row>
-    <row r="386" spans="1:3">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386"/>
       <c r="B386"/>
       <c r="C386"/>
     </row>
-    <row r="387" spans="1:3">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A387"/>
       <c r="B387"/>
       <c r="C387"/>
     </row>
-    <row r="388" spans="1:3" s="7" customFormat="1">
+    <row r="388" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A388"/>
       <c r="B388"/>
       <c r="C388"/>
     </row>
-    <row r="389" spans="1:3" s="7" customFormat="1">
+    <row r="389" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A389"/>
       <c r="B389"/>
       <c r="C389"/>
     </row>
-    <row r="390" spans="1:3" s="7" customFormat="1">
+    <row r="390" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A390"/>
       <c r="B390"/>
       <c r="C390"/>
     </row>
-    <row r="391" spans="1:3" s="7" customFormat="1">
+    <row r="391" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A391"/>
       <c r="B391"/>
       <c r="C391"/>
     </row>
-    <row r="392" spans="1:3" s="7" customFormat="1">
+    <row r="392" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A392"/>
       <c r="B392"/>
       <c r="C392"/>
     </row>
-    <row r="393" spans="1:3" s="7" customFormat="1">
+    <row r="393" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A393"/>
       <c r="B393"/>
       <c r="C393"/>
     </row>
-    <row r="394" spans="1:3" s="7" customFormat="1">
+    <row r="394" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A394"/>
       <c r="B394"/>
       <c r="C394"/>
     </row>
-    <row r="395" spans="1:3" s="7" customFormat="1">
+    <row r="395" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A395"/>
       <c r="B395"/>
       <c r="C395"/>
     </row>
-    <row r="396" spans="1:3" s="7" customFormat="1">
+    <row r="396" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A396"/>
       <c r="B396"/>
       <c r="C396"/>
     </row>
-    <row r="397" spans="1:3" s="7" customFormat="1">
+    <row r="397" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A397"/>
       <c r="B397"/>
       <c r="C397"/>
     </row>
-    <row r="398" spans="1:3">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398"/>
       <c r="B398"/>
       <c r="C398"/>
     </row>
-    <row r="399" spans="1:3">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399"/>
       <c r="B399"/>
       <c r="C399"/>
     </row>
-    <row r="400" spans="1:3">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400"/>
       <c r="B400"/>
       <c r="C400"/>
     </row>
-    <row r="401" spans="1:3">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401"/>
       <c r="B401"/>
       <c r="C401"/>
     </row>
-    <row r="402" spans="1:3">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402"/>
       <c r="B402"/>
       <c r="C402"/>
     </row>
-    <row r="403" spans="1:3">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403"/>
       <c r="B403"/>
       <c r="C403"/>
     </row>
-    <row r="404" spans="1:3">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404"/>
       <c r="B404"/>
       <c r="C404"/>
     </row>
-    <row r="405" spans="1:3">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405"/>
       <c r="B405"/>
       <c r="C405"/>
     </row>
-    <row r="406" spans="1:3">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406"/>
       <c r="B406"/>
       <c r="C406"/>
     </row>
-    <row r="407" spans="1:3">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407"/>
       <c r="B407"/>
       <c r="C407"/>
     </row>
-    <row r="408" spans="1:3">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408"/>
       <c r="B408"/>
       <c r="C408"/>
     </row>
-    <row r="409" spans="1:3">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409"/>
       <c r="B409"/>
       <c r="C409"/>
     </row>
-    <row r="410" spans="1:3">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410"/>
       <c r="B410"/>
       <c r="C410"/>
     </row>
-    <row r="411" spans="1:3">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411"/>
       <c r="B411"/>
       <c r="C411"/>
     </row>
-    <row r="412" spans="1:3">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412"/>
       <c r="B412"/>
       <c r="C412"/>
     </row>
-    <row r="413" spans="1:3">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413"/>
       <c r="B413"/>
       <c r="C413"/>
     </row>
-    <row r="414" spans="1:3">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414"/>
       <c r="B414"/>
       <c r="C414"/>
     </row>
-    <row r="415" spans="1:3">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415"/>
       <c r="B415"/>
       <c r="C415"/>
     </row>
-    <row r="416" spans="1:3">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416"/>
       <c r="B416"/>
       <c r="C416"/>
     </row>
-    <row r="417" spans="1:3">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417"/>
       <c r="B417"/>
       <c r="C417"/>
     </row>
-    <row r="418" spans="1:3">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418"/>
       <c r="B418"/>
       <c r="C418"/>
     </row>
-    <row r="419" spans="1:3">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419"/>
       <c r="B419"/>
       <c r="C419"/>
     </row>
-    <row r="420" spans="1:3">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420"/>
       <c r="B420"/>
       <c r="C420"/>
     </row>
-    <row r="421" spans="1:3">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421"/>
       <c r="B421"/>
       <c r="C421"/>
     </row>
-    <row r="422" spans="1:3">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422"/>
       <c r="B422"/>
       <c r="C422"/>
     </row>
-    <row r="423" spans="1:3">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423"/>
       <c r="B423"/>
       <c r="C423"/>
     </row>
-    <row r="424" spans="1:3">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424"/>
       <c r="B424"/>
       <c r="C424"/>
     </row>
-    <row r="425" spans="1:3">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425"/>
       <c r="B425"/>
       <c r="C425"/>
     </row>
-    <row r="426" spans="1:3">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426"/>
       <c r="B426"/>
       <c r="C426"/>
     </row>
-    <row r="427" spans="1:3">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427"/>
       <c r="B427"/>
       <c r="C427"/>
     </row>
-    <row r="428" spans="1:3">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428"/>
       <c r="B428"/>
       <c r="C428"/>
     </row>
-    <row r="429" spans="1:3">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429"/>
       <c r="B429"/>
       <c r="C429"/>
     </row>
-    <row r="430" spans="1:3">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430"/>
       <c r="B430"/>
       <c r="C430"/>
     </row>
-    <row r="431" spans="1:3">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431"/>
       <c r="B431"/>
       <c r="C431"/>
     </row>
-    <row r="432" spans="1:3" ht="14.5" customHeight="1">
+    <row r="432" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A432"/>
       <c r="B432"/>
       <c r="C432"/>
     </row>
-    <row r="433" spans="1:3" ht="14.5" customHeight="1">
+    <row r="433" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A433"/>
       <c r="B433"/>
       <c r="C433"/>
     </row>
-    <row r="434" spans="1:3" ht="14.5" customHeight="1">
+    <row r="434" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A434"/>
       <c r="B434"/>
       <c r="C434"/>
     </row>
-    <row r="435" spans="1:3" ht="14.5" customHeight="1">
+    <row r="435" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A435"/>
       <c r="B435"/>
       <c r="C435"/>
     </row>
-    <row r="436" spans="1:3" ht="14.5" customHeight="1">
+    <row r="436" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A436"/>
       <c r="B436"/>
       <c r="C436"/>
     </row>
-    <row r="437" spans="1:3" ht="14.5" customHeight="1">
+    <row r="437" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A437"/>
       <c r="B437"/>
       <c r="C437"/>
     </row>
-    <row r="438" spans="1:3" ht="14.5" customHeight="1">
+    <row r="438" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A438"/>
       <c r="B438"/>
       <c r="C438"/>
     </row>
-    <row r="439" spans="1:3" ht="14.5" customHeight="1">
+    <row r="439" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A439"/>
       <c r="B439"/>
       <c r="C439"/>
     </row>
-    <row r="440" spans="1:3" ht="14.5" customHeight="1">
+    <row r="440" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A440"/>
       <c r="B440"/>
       <c r="C440"/>
     </row>
-    <row r="441" spans="1:3" ht="14.5" customHeight="1">
+    <row r="441" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A441"/>
       <c r="B441"/>
       <c r="C441"/>
     </row>
-    <row r="442" spans="1:3" ht="14.5" customHeight="1">
+    <row r="442" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A442"/>
       <c r="B442"/>
       <c r="C442"/>
     </row>
-    <row r="443" spans="1:3" ht="14.5" customHeight="1">
+    <row r="443" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A443"/>
       <c r="B443"/>
       <c r="C443"/>
     </row>
-    <row r="444" spans="1:3">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444"/>
       <c r="B444"/>
       <c r="C444"/>
     </row>
-    <row r="445" spans="1:3">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A445"/>
       <c r="B445"/>
       <c r="C445"/>
     </row>
-    <row r="446" spans="1:3">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A446"/>
       <c r="B446"/>
       <c r="C446"/>
     </row>
-    <row r="447" spans="1:3">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A447"/>
       <c r="B447"/>
       <c r="C447"/>
     </row>
-    <row r="448" spans="1:3">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A448"/>
       <c r="B448"/>
       <c r="C448"/>
     </row>
-    <row r="449" spans="1:3">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A449"/>
       <c r="B449"/>
       <c r="C449"/>
     </row>
-    <row r="450" spans="1:3">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A450"/>
       <c r="B450"/>
       <c r="C450"/>
     </row>
-    <row r="451" spans="1:3">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A451"/>
       <c r="B451"/>
       <c r="C451"/>
     </row>
-    <row r="452" spans="1:3">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A452"/>
       <c r="B452"/>
       <c r="C452"/>
     </row>
-    <row r="453" spans="1:3">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A453"/>
       <c r="B453"/>
       <c r="C453"/>
     </row>
-    <row r="454" spans="1:3">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A454"/>
       <c r="B454"/>
       <c r="C454"/>
     </row>
-    <row r="455" spans="1:3">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A455"/>
       <c r="B455"/>
       <c r="C455"/>
     </row>
-    <row r="456" spans="1:3">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A456"/>
       <c r="B456"/>
       <c r="C456"/>
     </row>
-    <row r="457" spans="1:3">
+    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A457"/>
       <c r="B457"/>
       <c r="C457"/>
     </row>
-    <row r="458" spans="1:3">
+    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A458"/>
       <c r="B458"/>
       <c r="C458"/>
     </row>
-    <row r="459" spans="1:3">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A459"/>
       <c r="B459"/>
       <c r="C459"/>
     </row>
-    <row r="460" spans="1:3">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A460"/>
       <c r="B460"/>
       <c r="C460"/>
     </row>
-    <row r="461" spans="1:3">
+    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A461"/>
       <c r="B461"/>
       <c r="C461"/>
     </row>
-    <row r="462" spans="1:3">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A462"/>
       <c r="B462"/>
       <c r="C462"/>
     </row>
-    <row r="463" spans="1:3">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A463"/>
       <c r="B463"/>
       <c r="C463"/>
     </row>
-    <row r="464" spans="1:3">
+    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A464"/>
       <c r="B464"/>
       <c r="C464"/>
     </row>
-    <row r="465" spans="1:3">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A465"/>
       <c r="B465"/>
       <c r="C465"/>
     </row>
-    <row r="466" spans="1:3">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A466"/>
       <c r="B466"/>
       <c r="C466"/>
     </row>
-    <row r="467" spans="1:3" s="6" customFormat="1">
+    <row r="467" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A467"/>
       <c r="B467"/>
       <c r="C467"/>
     </row>
-    <row r="468" spans="1:3" s="6" customFormat="1">
+    <row r="468" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A468"/>
       <c r="B468"/>
       <c r="C468"/>
     </row>
-    <row r="469" spans="1:3" s="6" customFormat="1">
+    <row r="469" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A469"/>
       <c r="B469"/>
       <c r="C469"/>
     </row>
-    <row r="470" spans="1:3" s="6" customFormat="1">
+    <row r="470" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A470"/>
       <c r="B470"/>
       <c r="C470"/>
     </row>
-    <row r="471" spans="1:3" s="6" customFormat="1">
+    <row r="471" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A471"/>
       <c r="B471"/>
       <c r="C471"/>
     </row>
-    <row r="472" spans="1:3" s="6" customFormat="1">
+    <row r="472" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A472"/>
       <c r="B472"/>
       <c r="C472"/>
     </row>
-    <row r="473" spans="1:3" s="6" customFormat="1">
+    <row r="473" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A473"/>
       <c r="B473"/>
       <c r="C473"/>
     </row>
-    <row r="474" spans="1:3" s="6" customFormat="1">
+    <row r="474" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A474"/>
       <c r="B474"/>
       <c r="C474"/>
     </row>
-    <row r="475" spans="1:3" s="6" customFormat="1">
+    <row r="475" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A475"/>
       <c r="B475"/>
       <c r="C475"/>
     </row>
-    <row r="476" spans="1:3" s="6" customFormat="1">
+    <row r="476" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A476"/>
       <c r="B476"/>
       <c r="C476"/>
     </row>
-    <row r="477" spans="1:3" s="6" customFormat="1">
+    <row r="477" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A477"/>
       <c r="B477"/>
       <c r="C477"/>
     </row>
-    <row r="478" spans="1:3" s="6" customFormat="1">
+    <row r="478" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A478"/>
       <c r="B478"/>
       <c r="C478"/>
     </row>
-    <row r="479" spans="1:3" s="6" customFormat="1">
+    <row r="479" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A479"/>
       <c r="B479"/>
       <c r="C479"/>
     </row>
-    <row r="480" spans="1:3" s="6" customFormat="1">
+    <row r="480" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A480"/>
       <c r="B480"/>
       <c r="C480"/>
     </row>
-    <row r="481" spans="1:3" s="6" customFormat="1">
+    <row r="481" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A481"/>
       <c r="B481"/>
       <c r="C481"/>
     </row>
-    <row r="482" spans="1:3" s="6" customFormat="1">
+    <row r="482" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A482"/>
       <c r="B482"/>
       <c r="C482"/>
     </row>
-    <row r="483" spans="1:3" s="6" customFormat="1">
+    <row r="483" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A483"/>
       <c r="B483"/>
       <c r="C483"/>
     </row>
-    <row r="484" spans="1:3" s="6" customFormat="1">
+    <row r="484" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A484"/>
       <c r="B484"/>
       <c r="C484"/>
     </row>
-    <row r="485" spans="1:3" s="6" customFormat="1">
+    <row r="485" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A485"/>
       <c r="B485"/>
       <c r="C485"/>
     </row>
-    <row r="486" spans="1:3" s="6" customFormat="1">
+    <row r="486" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A486"/>
       <c r="B486"/>
       <c r="C486"/>
     </row>
-    <row r="487" spans="1:3" s="6" customFormat="1">
+    <row r="487" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A487"/>
       <c r="B487"/>
       <c r="C487"/>
     </row>
-    <row r="488" spans="1:3" s="6" customFormat="1">
+    <row r="488" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A488"/>
       <c r="B488"/>
       <c r="C488"/>
     </row>
-    <row r="489" spans="1:3" s="6" customFormat="1">
+    <row r="489" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A489"/>
       <c r="B489"/>
       <c r="C489"/>
     </row>
-    <row r="490" spans="1:3" s="6" customFormat="1">
+    <row r="490" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A490"/>
       <c r="B490"/>
       <c r="C490"/>
     </row>
-    <row r="491" spans="1:3" s="6" customFormat="1">
+    <row r="491" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A491"/>
       <c r="B491"/>
       <c r="C491"/>
     </row>
-    <row r="492" spans="1:3" s="6" customFormat="1">
+    <row r="492" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A492"/>
       <c r="B492"/>
       <c r="C492"/>
     </row>
-    <row r="493" spans="1:3" s="6" customFormat="1">
+    <row r="493" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A493"/>
       <c r="B493"/>
       <c r="C493"/>
     </row>
-    <row r="494" spans="1:3" s="6" customFormat="1">
+    <row r="494" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A494"/>
       <c r="B494"/>
       <c r="C494"/>
     </row>
-    <row r="495" spans="1:3" s="6" customFormat="1">
+    <row r="495" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A495"/>
       <c r="B495"/>
       <c r="C495"/>
     </row>
-    <row r="496" spans="1:3" s="6" customFormat="1">
+    <row r="496" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A496"/>
       <c r="B496"/>
       <c r="C496"/>
     </row>
-    <row r="497" spans="1:3" s="6" customFormat="1">
+    <row r="497" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A497"/>
       <c r="B497"/>
       <c r="C497"/>
     </row>
-    <row r="498" spans="1:3" s="6" customFormat="1">
+    <row r="498" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A498"/>
       <c r="B498"/>
       <c r="C498"/>
     </row>
-    <row r="499" spans="1:3" s="6" customFormat="1">
+    <row r="499" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A499"/>
       <c r="B499"/>
       <c r="C499"/>
     </row>
-    <row r="500" spans="1:3" s="6" customFormat="1">
+    <row r="500" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A500"/>
       <c r="B500"/>
       <c r="C500"/>
     </row>
-    <row r="501" spans="1:3" s="6" customFormat="1">
+    <row r="501" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A501"/>
       <c r="B501"/>
       <c r="C501"/>
     </row>
-    <row r="502" spans="1:3" s="6" customFormat="1">
+    <row r="502" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A502"/>
       <c r="B502"/>
       <c r="C502"/>
     </row>
-    <row r="503" spans="1:3" s="6" customFormat="1">
+    <row r="503" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A503"/>
       <c r="B503"/>
       <c r="C503"/>
     </row>
-    <row r="504" spans="1:3" s="6" customFormat="1">
+    <row r="504" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A504"/>
       <c r="B504"/>
       <c r="C504"/>
     </row>
-    <row r="505" spans="1:3" s="6" customFormat="1">
+    <row r="505" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A505"/>
       <c r="B505"/>
       <c r="C505"/>
     </row>
-    <row r="506" spans="1:3" s="6" customFormat="1">
+    <row r="506" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A506"/>
       <c r="B506"/>
       <c r="C506"/>
     </row>
-    <row r="507" spans="1:3" s="6" customFormat="1">
+    <row r="507" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A507"/>
       <c r="B507"/>
       <c r="C507"/>
     </row>
-    <row r="508" spans="1:3" s="6" customFormat="1">
+    <row r="508" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A508"/>
       <c r="B508"/>
       <c r="C508"/>
     </row>
-    <row r="509" spans="1:3" s="6" customFormat="1">
+    <row r="509" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A509"/>
       <c r="B509"/>
       <c r="C509"/>
     </row>
-    <row r="510" spans="1:3" s="6" customFormat="1">
+    <row r="510" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A510"/>
       <c r="B510"/>
       <c r="C510"/>
     </row>
-    <row r="511" spans="1:3" s="6" customFormat="1">
+    <row r="511" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A511"/>
       <c r="B511"/>
       <c r="C511"/>
     </row>
-    <row r="512" spans="1:3" s="6" customFormat="1">
+    <row r="512" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A512"/>
       <c r="B512"/>
       <c r="C512"/>
     </row>
-    <row r="513" spans="1:3" s="6" customFormat="1">
+    <row r="513" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A513"/>
       <c r="B513"/>
       <c r="C513"/>
     </row>
-    <row r="514" spans="1:3" s="6" customFormat="1">
+    <row r="514" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A514"/>
       <c r="B514"/>
       <c r="C514"/>
     </row>
-    <row r="515" spans="1:3" s="6" customFormat="1">
+    <row r="515" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A515"/>
       <c r="B515"/>
       <c r="C515"/>
     </row>
-    <row r="516" spans="1:3" s="6" customFormat="1">
+    <row r="516" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A516"/>
       <c r="B516"/>
       <c r="C516"/>
     </row>
-    <row r="517" spans="1:3" s="6" customFormat="1">
+    <row r="517" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A517"/>
       <c r="B517"/>
       <c r="C517"/>
     </row>
-    <row r="518" spans="1:3" s="6" customFormat="1">
+    <row r="518" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A518"/>
       <c r="B518"/>
       <c r="C518"/>
     </row>
-    <row r="519" spans="1:3" s="6" customFormat="1">
+    <row r="519" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A519"/>
       <c r="B519"/>
       <c r="C519"/>
     </row>
-    <row r="520" spans="1:3" s="6" customFormat="1">
+    <row r="520" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A520"/>
       <c r="B520"/>
       <c r="C520"/>
     </row>
-    <row r="521" spans="1:3" s="6" customFormat="1">
+    <row r="521" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A521"/>
       <c r="B521"/>
       <c r="C521"/>
     </row>
-    <row r="522" spans="1:3" s="6" customFormat="1">
+    <row r="522" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A522"/>
       <c r="B522"/>
       <c r="C522"/>
     </row>
-    <row r="523" spans="1:3" s="6" customFormat="1">
+    <row r="523" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A523"/>
       <c r="B523"/>
       <c r="C523"/>
     </row>
-    <row r="524" spans="1:3" s="6" customFormat="1">
+    <row r="524" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A524"/>
       <c r="B524"/>
       <c r="C524"/>
     </row>
-    <row r="525" spans="1:3" s="6" customFormat="1">
+    <row r="525" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A525"/>
       <c r="B525"/>
       <c r="C525"/>
     </row>
-    <row r="526" spans="1:3" s="6" customFormat="1">
+    <row r="526" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A526"/>
       <c r="B526"/>
       <c r="C526"/>
     </row>
-    <row r="527" spans="1:3" s="6" customFormat="1">
+    <row r="527" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A527"/>
       <c r="B527"/>
       <c r="C527"/>
     </row>
-    <row r="528" spans="1:3" s="6" customFormat="1">
+    <row r="528" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A528"/>
       <c r="B528"/>
       <c r="C528"/>
     </row>
-    <row r="529" spans="1:3" s="6" customFormat="1">
+    <row r="529" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A529"/>
       <c r="B529"/>
       <c r="C529"/>
     </row>
-    <row r="530" spans="1:3" s="6" customFormat="1">
+    <row r="530" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A530"/>
       <c r="B530"/>
       <c r="C530"/>
     </row>
-    <row r="531" spans="1:3" s="6" customFormat="1">
+    <row r="531" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A531"/>
       <c r="B531"/>
       <c r="C531"/>
     </row>
-    <row r="532" spans="1:3" s="6" customFormat="1">
+    <row r="532" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A532"/>
       <c r="B532"/>
       <c r="C532"/>
     </row>
-    <row r="533" spans="1:3" s="6" customFormat="1">
+    <row r="533" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A533"/>
       <c r="B533"/>
       <c r="C533"/>
     </row>
-    <row r="534" spans="1:3" s="6" customFormat="1">
+    <row r="534" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A534"/>
       <c r="B534"/>
       <c r="C534"/>
     </row>
-    <row r="535" spans="1:3" s="6" customFormat="1">
+    <row r="535" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A535"/>
       <c r="B535"/>
       <c r="C535"/>
     </row>
-    <row r="536" spans="1:3" s="6" customFormat="1">
+    <row r="536" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A536"/>
       <c r="B536"/>
       <c r="C536"/>
     </row>
-    <row r="537" spans="1:3" s="6" customFormat="1">
+    <row r="537" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A537"/>
       <c r="B537"/>
       <c r="C537"/>
     </row>
-    <row r="538" spans="1:3" s="6" customFormat="1">
+    <row r="538" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A538"/>
       <c r="B538"/>
       <c r="C538"/>
     </row>
-    <row r="539" spans="1:3" s="6" customFormat="1">
+    <row r="539" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A539"/>
       <c r="B539"/>
       <c r="C539"/>
     </row>
-    <row r="540" spans="1:3" s="6" customFormat="1">
+    <row r="540" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A540"/>
       <c r="B540"/>
       <c r="C540"/>
     </row>
-    <row r="541" spans="1:3" s="6" customFormat="1">
+    <row r="541" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A541"/>
       <c r="B541"/>
       <c r="C541"/>
     </row>
-    <row r="542" spans="1:3" s="6" customFormat="1">
+    <row r="542" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A542"/>
       <c r="B542"/>
       <c r="C542"/>
     </row>
-    <row r="543" spans="1:3" s="6" customFormat="1">
+    <row r="543" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A543"/>
       <c r="B543"/>
       <c r="C543"/>
     </row>
-    <row r="544" spans="1:3" s="6" customFormat="1">
+    <row r="544" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A544"/>
       <c r="B544"/>
       <c r="C544"/>
     </row>
-    <row r="545" spans="1:3" s="6" customFormat="1">
+    <row r="545" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A545"/>
       <c r="B545"/>
       <c r="C545"/>
     </row>
-    <row r="546" spans="1:3" s="6" customFormat="1">
+    <row r="546" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A546"/>
       <c r="B546"/>
       <c r="C546"/>
     </row>
-    <row r="547" spans="1:3" s="6" customFormat="1">
+    <row r="547" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A547"/>
       <c r="B547"/>
       <c r="C547"/>
     </row>
-    <row r="548" spans="1:3" s="6" customFormat="1">
+    <row r="548" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A548"/>
       <c r="B548"/>
       <c r="C548"/>
     </row>
-    <row r="549" spans="1:3" s="6" customFormat="1">
+    <row r="549" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A549"/>
       <c r="B549"/>
       <c r="C549"/>
     </row>
-    <row r="550" spans="1:3" s="6" customFormat="1">
+    <row r="550" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A550"/>
       <c r="B550"/>
       <c r="C550"/>
     </row>
-    <row r="551" spans="1:3" s="6" customFormat="1">
+    <row r="551" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A551"/>
       <c r="B551"/>
       <c r="C551"/>
     </row>
-    <row r="552" spans="1:3" s="6" customFormat="1">
+    <row r="552" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A552"/>
       <c r="B552"/>
       <c r="C552"/>
     </row>
-    <row r="553" spans="1:3" s="6" customFormat="1">
+    <row r="553" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A553"/>
       <c r="B553"/>
       <c r="C553"/>
     </row>
-    <row r="554" spans="1:3" s="6" customFormat="1">
+    <row r="554" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A554"/>
       <c r="B554"/>
       <c r="C554"/>
     </row>
-    <row r="555" spans="1:3" s="6" customFormat="1">
+    <row r="555" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A555"/>
       <c r="B555"/>
       <c r="C555"/>
     </row>
-    <row r="556" spans="1:3" s="6" customFormat="1">
+    <row r="556" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A556"/>
       <c r="B556"/>
       <c r="C556"/>
     </row>
-    <row r="557" spans="1:3" s="8" customFormat="1">
+    <row r="557" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A557"/>
       <c r="B557"/>
       <c r="C557"/>
     </row>
-    <row r="558" spans="1:3" s="8" customFormat="1">
+    <row r="558" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A558"/>
       <c r="B558"/>
       <c r="C558"/>
     </row>
-    <row r="559" spans="1:3" s="8" customFormat="1">
+    <row r="559" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A559"/>
       <c r="B559"/>
       <c r="C559"/>
     </row>
-    <row r="560" spans="1:3" s="8" customFormat="1">
+    <row r="560" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A560"/>
       <c r="B560"/>
       <c r="C560"/>
     </row>
-    <row r="561" spans="1:3" s="8" customFormat="1">
+    <row r="561" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A561"/>
       <c r="B561"/>
       <c r="C561"/>
     </row>
-    <row r="562" spans="1:3" s="8" customFormat="1">
+    <row r="562" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A562"/>
       <c r="B562"/>
       <c r="C562"/>
     </row>
-    <row r="563" spans="1:3" s="8" customFormat="1">
+    <row r="563" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A563"/>
       <c r="B563"/>
       <c r="C563"/>
     </row>
-    <row r="564" spans="1:3" s="8" customFormat="1">
+    <row r="564" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A564"/>
       <c r="B564"/>
       <c r="C564"/>
     </row>
-    <row r="565" spans="1:3" s="8" customFormat="1">
+    <row r="565" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A565"/>
       <c r="B565"/>
       <c r="C565"/>
     </row>
-    <row r="566" spans="1:3" s="8" customFormat="1">
+    <row r="566" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A566"/>
       <c r="B566"/>
       <c r="C566"/>
     </row>
-    <row r="567" spans="1:3" s="8" customFormat="1">
+    <row r="567" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A567"/>
       <c r="B567"/>
       <c r="C567"/>
     </row>
-    <row r="568" spans="1:3" s="8" customFormat="1">
+    <row r="568" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A568"/>
       <c r="B568"/>
       <c r="C568"/>
     </row>
-    <row r="569" spans="1:3" s="8" customFormat="1">
+    <row r="569" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A569"/>
       <c r="B569"/>
       <c r="C569"/>
     </row>
-    <row r="570" spans="1:3" s="8" customFormat="1">
+    <row r="570" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A570"/>
       <c r="B570"/>
       <c r="C570"/>
     </row>
-    <row r="571" spans="1:3" s="8" customFormat="1">
+    <row r="571" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A571"/>
       <c r="B571"/>
       <c r="C571"/>
     </row>
-    <row r="572" spans="1:3" s="8" customFormat="1">
+    <row r="572" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A572"/>
       <c r="B572"/>
       <c r="C572"/>
     </row>
-    <row r="573" spans="1:3" s="8" customFormat="1">
+    <row r="573" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A573"/>
       <c r="B573"/>
       <c r="C573"/>
     </row>
-    <row r="574" spans="1:3" s="8" customFormat="1">
+    <row r="574" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A574"/>
       <c r="B574"/>
       <c r="C574"/>
     </row>
-    <row r="575" spans="1:3" s="8" customFormat="1">
+    <row r="575" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A575"/>
       <c r="B575"/>
       <c r="C575"/>
     </row>
-    <row r="576" spans="1:3" s="8" customFormat="1">
+    <row r="576" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A576"/>
       <c r="B576"/>
       <c r="C576"/>
     </row>
-    <row r="577" spans="1:3" s="8" customFormat="1">
+    <row r="577" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A577"/>
       <c r="B577"/>
       <c r="C577"/>
     </row>
-    <row r="578" spans="1:3" s="8" customFormat="1">
+    <row r="578" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A578"/>
       <c r="B578"/>
       <c r="C578"/>
     </row>
-    <row r="579" spans="1:3" s="8" customFormat="1">
+    <row r="579" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A579"/>
       <c r="B579"/>
       <c r="C579"/>
     </row>
-    <row r="580" spans="1:3" s="8" customFormat="1">
+    <row r="580" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A580"/>
       <c r="B580"/>
       <c r="C580"/>
     </row>
-    <row r="581" spans="1:3">
+    <row r="581" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A581"/>
       <c r="B581"/>
       <c r="C581"/>
     </row>
-    <row r="582" spans="1:3">
+    <row r="582" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A582"/>
       <c r="B582"/>
       <c r="C582"/>
     </row>
-    <row r="583" spans="1:3">
+    <row r="583" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A583"/>
       <c r="B583"/>
       <c r="C583"/>
     </row>
-    <row r="584" spans="1:3">
+    <row r="584" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A584"/>
       <c r="B584"/>
       <c r="C584"/>
     </row>
-    <row r="585" spans="1:3">
+    <row r="585" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A585"/>
       <c r="B585"/>
       <c r="C585"/>
     </row>
-    <row r="586" spans="1:3">
+    <row r="586" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A586"/>
       <c r="B586"/>
       <c r="C586"/>
     </row>
-    <row r="587" spans="1:3">
+    <row r="587" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A587"/>
       <c r="B587"/>
       <c r="C587"/>
     </row>
-    <row r="588" spans="1:3">
+    <row r="588" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A588"/>
       <c r="B588"/>
       <c r="C588"/>
     </row>
-    <row r="589" spans="1:3">
+    <row r="589" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A589"/>
       <c r="B589"/>
       <c r="C589"/>
     </row>
-    <row r="590" spans="1:3">
+    <row r="590" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A590"/>
       <c r="B590"/>
       <c r="C590"/>
     </row>
-    <row r="591" spans="1:3">
+    <row r="591" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A591"/>
       <c r="B591"/>
       <c r="C591"/>
     </row>
-    <row r="592" spans="1:3">
+    <row r="592" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A592"/>
       <c r="B592"/>
       <c r="C592"/>
     </row>
-    <row r="593" spans="1:3">
+    <row r="593" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A593"/>
       <c r="B593"/>
       <c r="C593"/>
     </row>
-    <row r="594" spans="1:3">
+    <row r="594" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A594"/>
       <c r="B594"/>
       <c r="C594"/>
     </row>
-    <row r="595" spans="1:3">
+    <row r="595" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A595"/>
       <c r="B595"/>
       <c r="C595"/>
     </row>
-    <row r="596" spans="1:3">
+    <row r="596" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A596"/>
       <c r="B596"/>
       <c r="C596"/>
     </row>
-    <row r="597" spans="1:3">
+    <row r="597" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A597"/>
       <c r="B597"/>
       <c r="C597"/>
     </row>
-    <row r="598" spans="1:3">
+    <row r="598" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A598"/>
       <c r="B598"/>
       <c r="C598"/>
     </row>
-    <row r="599" spans="1:3">
+    <row r="599" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A599"/>
       <c r="B599"/>
       <c r="C599"/>
     </row>
-    <row r="600" spans="1:3">
+    <row r="600" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A600"/>
       <c r="B600"/>
       <c r="C600"/>
     </row>
-    <row r="601" spans="1:3">
+    <row r="601" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A601"/>
       <c r="B601"/>
       <c r="C601"/>
     </row>
-    <row r="602" spans="1:3">
+    <row r="602" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A602"/>
       <c r="B602"/>
       <c r="C602"/>
     </row>
-    <row r="603" spans="1:3">
+    <row r="603" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A603"/>
       <c r="B603"/>
       <c r="C603"/>
     </row>
-    <row r="604" spans="1:3">
+    <row r="604" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A604"/>
       <c r="B604"/>
       <c r="C604"/>
     </row>
-    <row r="605" spans="1:3">
+    <row r="605" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A605"/>
       <c r="B605"/>
       <c r="C605"/>
     </row>
-    <row r="606" spans="1:3">
+    <row r="606" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A606"/>
       <c r="B606"/>
       <c r="C606"/>
     </row>
-    <row r="607" spans="1:3">
+    <row r="607" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A607"/>
       <c r="B607"/>
       <c r="C607"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C177" xr:uid="{F0F1E9AA-42FA-48CE-9C0D-6753CE8DE448}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="jtgh_11"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C177" xr:uid="{F0F1E9AA-42FA-48CE-9C0D-6753CE8DE448}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C1048576" xr:uid="{282CD8DC-1CD6-4FEE-88BD-6500CF45AFA3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C1048576 D3:D14" xr:uid="{282CD8DC-1CD6-4FEE-88BD-6500CF45AFA3}">
       <formula1>"#na, stage_1, stage_2, stage_3, stage_4, stage_5, stage_6, stage_7, stage_8, stage_9, stage_10, stage_11, stage_12, stage_13"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>